<commit_message>
worked on household indicators
</commit_message>
<xml_diff>
--- a/forms/app/moh_515_post_outbreak.xlsx
+++ b/forms/app/moh_515_post_outbreak.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>type</t>
   </si>
@@ -42,7 +42,7 @@
     <t>begin group</t>
   </si>
   <si>
-    <t>inputs</t>
+    <t>form_summary</t>
   </si>
   <si>
     <t>Form Summary</t>
@@ -54,7 +54,7 @@
     <t>cha_name</t>
   </si>
   <si>
-    <t>What is your name?</t>
+    <t>What Is Your Name?</t>
   </si>
   <si>
     <t>yes</t>
@@ -69,19 +69,19 @@
     <t>cha_area</t>
   </si>
   <si>
-    <t>What is your area?</t>
+    <t>What Is Your Area?</t>
   </si>
   <si>
     <t>cha_facility</t>
   </si>
   <si>
-    <t>What is your linked facility?</t>
+    <t>What Is Your Linked Facility?</t>
   </si>
   <si>
     <t>cha_county</t>
   </si>
   <si>
-    <t>What county do you belong to?</t>
+    <t>What County Do You Belong To?</t>
   </si>
   <si>
     <t>integer</t>
@@ -90,7 +90,7 @@
     <t>chp_total</t>
   </si>
   <si>
-    <t>How many CHPs are in your area?</t>
+    <t>How Many CHPs Are In Your Area?</t>
   </si>
   <si>
     <t>numbers</t>
@@ -99,10 +99,46 @@
     <t>chp_reported_total</t>
   </si>
   <si>
-    <t>How many CHPs submitted report?</t>
+    <t>How Many CHPs Submitted Monthly Report?</t>
   </si>
   <si>
     <t>end group</t>
+  </si>
+  <si>
+    <t>household_indicators</t>
+  </si>
+  <si>
+    <t>Household Indicators</t>
+  </si>
+  <si>
+    <t>total_households</t>
+  </si>
+  <si>
+    <t>Total Households In The Area?</t>
+  </si>
+  <si>
+    <t>new_households</t>
+  </si>
+  <si>
+    <t>Number Of New Households Registered This Month?</t>
+  </si>
+  <si>
+    <t>new_households_visited</t>
+  </si>
+  <si>
+    <t>Number Of New Households Visited This Month?</t>
+  </si>
+  <si>
+    <t>new_households_with_clean_water</t>
+  </si>
+  <si>
+    <t>Number Of New Households Visited This Month With Clean Water Access?</t>
+  </si>
+  <si>
+    <t>new_households_with_latrines</t>
+  </si>
+  <si>
+    <t>Number Of New Households Visited This Month With Latrines/Toilets?</t>
   </si>
   <si>
     <t>form_title</t>
@@ -410,7 +446,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="29.63"/>
+    <col customWidth="1" min="2" max="2" width="18.88"/>
+    <col customWidth="1" min="3" max="3" width="60.13"/>
     <col customWidth="1" min="8" max="8" width="25.13"/>
   </cols>
   <sheetData>
@@ -551,6 +588,101 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -594,36 +726,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cholera cases group
</commit_message>
<xml_diff>
--- a/forms/app/moh_515_post_outbreak.xlsx
+++ b/forms/app/moh_515_post_outbreak.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>type</t>
   </si>
@@ -139,6 +139,45 @@
   </si>
   <si>
     <t>Number Of New Households Visited This Month With Latrines/Toilets?</t>
+  </si>
+  <si>
+    <t>cholera_cases</t>
+  </si>
+  <si>
+    <t>Cholera Cases</t>
+  </si>
+  <si>
+    <t>num_screened</t>
+  </si>
+  <si>
+    <t>Number Of Persons Screened For Cholera</t>
+  </si>
+  <si>
+    <t>num_referred</t>
+  </si>
+  <si>
+    <t>Number Of Presumptive Cholera Persons Referred For Diagnosis</t>
+  </si>
+  <si>
+    <t>num_referred_reached</t>
+  </si>
+  <si>
+    <t>Number Of Referred Persons Who Reached Health Facility</t>
+  </si>
+  <si>
+    <t>${num_referred} &gt;0</t>
+  </si>
+  <si>
+    <t>num_confirmed_cases</t>
+  </si>
+  <si>
+    <t>Number Of Confirmed Cholera Cases At Health Facility</t>
+  </si>
+  <si>
+    <t>num_deaths</t>
+  </si>
+  <si>
+    <t>Number Of Deaths Due To Cholera In The Month</t>
   </si>
   <si>
     <t>form_title</t>
@@ -448,6 +487,7 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="18.88"/>
     <col customWidth="1" min="3" max="3" width="60.13"/>
+    <col customWidth="1" min="5" max="5" width="22.0"/>
     <col customWidth="1" min="8" max="8" width="25.13"/>
   </cols>
   <sheetData>
@@ -683,6 +723,112 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -726,36 +872,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed reference to CHA's name and area
</commit_message>
<xml_diff>
--- a/forms/app/moh_515_post_outbreak.xlsx
+++ b/forms/app/moh_515_post_outbreak.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="74">
   <si>
     <t>type</t>
   </si>
@@ -42,42 +42,42 @@
     <t>begin group</t>
   </si>
   <si>
+    <t>hidden_inputs</t>
+  </si>
+  <si>
+    <t>./source='user'</t>
+  </si>
+  <si>
+    <t>field-list</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>end group</t>
+  </si>
+  <si>
     <t>form_summary</t>
   </si>
   <si>
     <t>Form Summary</t>
   </si>
   <si>
-    <t>db:person</t>
-  </si>
-  <si>
-    <t>cha_name</t>
-  </si>
-  <si>
-    <t>What Is Your Name?</t>
+    <t>text</t>
+  </si>
+  <si>
+    <t>cha_facility</t>
+  </si>
+  <si>
+    <t>What Is Your Linked Facility?</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>db-object</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>cha_area</t>
-  </si>
-  <si>
-    <t>What Is Your Area?</t>
-  </si>
-  <si>
-    <t>cha_facility</t>
-  </si>
-  <si>
-    <t>What Is Your Linked Facility?</t>
-  </si>
-  <si>
     <t>cha_county</t>
   </si>
   <si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>How Many CHPs Submitted Monthly Report?</t>
-  </si>
-  <si>
-    <t>end group</t>
   </si>
   <si>
     <t>household_indicators</t>
@@ -554,91 +551,78 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -646,13 +630,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>26</v>
@@ -666,44 +650,47 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -711,13 +698,13 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>26</v>
@@ -734,13 +721,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>26</v>
@@ -757,13 +744,22 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -771,57 +767,50 @@
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>31</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -829,15 +818,15 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -852,16 +841,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>26</v>
@@ -878,13 +864,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>26</v>
@@ -901,13 +890,13 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>26</v>
@@ -921,44 +910,47 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
@@ -966,21 +958,21 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H26" s="2" t="s">
+      <c r="G26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -989,13 +981,13 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>26</v>
@@ -1009,10 +1001,33 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1055,36 +1070,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fine grained referred versus reached constraints
</commit_message>
<xml_diff>
--- a/forms/app/moh_515_post_outbreak.xlsx
+++ b/forms/app/moh_515_post_outbreak.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="90">
   <si>
     <t>type</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>${num_referred} &gt;0</t>
+  </si>
+  <si>
+    <t>.&lt;=${num_referred}</t>
+  </si>
+  <si>
+    <t>Number cannot exceed those referred</t>
   </si>
   <si>
     <t>num_confirmed_cases</t>
@@ -980,10 +986,10 @@
         <v>31</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24">
@@ -991,10 +997,10 @@
         <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>25</v>
@@ -1014,10 +1020,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>25</v>
@@ -1045,10 +1051,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
@@ -1059,10 +1065,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>25</v>
@@ -1082,10 +1088,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>25</v>
@@ -1105,10 +1111,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>25</v>
@@ -1128,7 +1134,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1171,36 +1177,36 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>